<commit_message>
Fix things to work with stock-by-sex and stock-by-age
Made a lot of modifications to the code so that the gsi_sim stuff would work with the ".." naming convention for stock subgroups.  I also updated the data files to use that naming convention.

Closed these to things on the TODO list:
0. Modify all the StockSex and StockAge xlsx files to use the ".." naming convention
0. Add a function or a few lines to check the originnames to make sure that if there are
</commit_message>
<xml_diff>
--- a/inst/data_files/CH11SIMPOP_StockAge.xlsx
+++ b/inst/data_files/CH11SIMPOP_StockAge.xlsx
@@ -1,15 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24526"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-3735" yWindow="-75" windowWidth="20115" windowHeight="7485"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="36980" windowHeight="21740"/>
   </bookViews>
   <sheets>
     <sheet name="chkSmooth" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -40,109 +45,109 @@
     <t>PWhandled</t>
   </si>
   <si>
-    <t>BY05UPSALM</t>
-  </si>
-  <si>
-    <t>BY06UPSALM</t>
-  </si>
-  <si>
-    <t>BY07UPSALM</t>
-  </si>
-  <si>
-    <t>BY08UPSALM</t>
-  </si>
-  <si>
-    <t>BY09UPSALM</t>
-  </si>
-  <si>
-    <t>BY05MFSALM</t>
-  </si>
-  <si>
-    <t>BY06MFSALM</t>
-  </si>
-  <si>
-    <t>BY07MFSALM</t>
-  </si>
-  <si>
-    <t>BY08MFSALM</t>
-  </si>
-  <si>
-    <t>BY09MFSALM</t>
-  </si>
-  <si>
-    <t>BY05CHMBLN</t>
-  </si>
-  <si>
-    <t>BY06CHMBLN</t>
-  </si>
-  <si>
-    <t>BY07CHMBLN</t>
-  </si>
-  <si>
-    <t>BY08CHMBLN</t>
-  </si>
-  <si>
-    <t>BY09CHMBLN</t>
-  </si>
-  <si>
-    <t>BY05SFSALM</t>
-  </si>
-  <si>
-    <t>BY06SFSALM</t>
-  </si>
-  <si>
-    <t>BY07SFSALM</t>
-  </si>
-  <si>
-    <t>BY08SFSALM</t>
-  </si>
-  <si>
-    <t>BY09SFSALM</t>
-  </si>
-  <si>
-    <t>BY05HELLSC</t>
-  </si>
-  <si>
-    <t>BY06HELLSC</t>
-  </si>
-  <si>
-    <t>BY07HELLSC</t>
-  </si>
-  <si>
-    <t>BY08HELLSC</t>
-  </si>
-  <si>
-    <t>BY09HELLSC</t>
-  </si>
-  <si>
-    <t>BY05TUCANO</t>
-  </si>
-  <si>
-    <t>BY06TUCANO</t>
-  </si>
-  <si>
-    <t>BY07TUCANO</t>
-  </si>
-  <si>
-    <t>BY08TUCANO</t>
-  </si>
-  <si>
-    <t>BY09TUCANO</t>
-  </si>
-  <si>
-    <t>BY05FALL</t>
-  </si>
-  <si>
-    <t>BY06FALL</t>
-  </si>
-  <si>
-    <t>BY07FALL</t>
-  </si>
-  <si>
-    <t>BY08FALL</t>
-  </si>
-  <si>
-    <t>BY09FALL</t>
+    <t>UPSALM..BY05</t>
+  </si>
+  <si>
+    <t>UPSALM..BY06</t>
+  </si>
+  <si>
+    <t>UPSALM..BY07</t>
+  </si>
+  <si>
+    <t>UPSALM..BY08</t>
+  </si>
+  <si>
+    <t>UPSALM..BY09</t>
+  </si>
+  <si>
+    <t>MFSALM..BY05</t>
+  </si>
+  <si>
+    <t>MFSALM..BY06</t>
+  </si>
+  <si>
+    <t>MFSALM..BY07</t>
+  </si>
+  <si>
+    <t>MFSALM..BY08</t>
+  </si>
+  <si>
+    <t>MFSALM..BY09</t>
+  </si>
+  <si>
+    <t>CHMBLN..BY05</t>
+  </si>
+  <si>
+    <t>CHMBLN..BY06</t>
+  </si>
+  <si>
+    <t>CHMBLN..BY07</t>
+  </si>
+  <si>
+    <t>CHMBLN..BY08</t>
+  </si>
+  <si>
+    <t>CHMBLN..BY09</t>
+  </si>
+  <si>
+    <t>SFSALM..BY05</t>
+  </si>
+  <si>
+    <t>SFSALM..BY06</t>
+  </si>
+  <si>
+    <t>SFSALM..BY07</t>
+  </si>
+  <si>
+    <t>SFSALM..BY08</t>
+  </si>
+  <si>
+    <t>SFSALM..BY09</t>
+  </si>
+  <si>
+    <t>HELLSC..BY05</t>
+  </si>
+  <si>
+    <t>HELLSC..BY06</t>
+  </si>
+  <si>
+    <t>HELLSC..BY07</t>
+  </si>
+  <si>
+    <t>HELLSC..BY08</t>
+  </si>
+  <si>
+    <t>HELLSC..BY09</t>
+  </si>
+  <si>
+    <t>TUCANO..BY05</t>
+  </si>
+  <si>
+    <t>TUCANO..BY06</t>
+  </si>
+  <si>
+    <t>TUCANO..BY07</t>
+  </si>
+  <si>
+    <t>TUCANO..BY08</t>
+  </si>
+  <si>
+    <t>TUCANO..BY09</t>
+  </si>
+  <si>
+    <t>FALL..BY05</t>
+  </si>
+  <si>
+    <t>FALL..BY06</t>
+  </si>
+  <si>
+    <t>FALL..BY07</t>
+  </si>
+  <si>
+    <t>FALL..BY08</t>
+  </si>
+  <si>
+    <t>FALL..BY09</t>
   </si>
 </sst>
 </file>
@@ -153,7 +158,7 @@
     <numFmt numFmtId="164" formatCode="0.0%"/>
     <numFmt numFmtId="165" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -301,6 +306,22 @@
       <name val="Consolas"/>
       <family val="3"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -599,7 +620,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="43">
+  <cellStyleXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -643,6 +664,8 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -668,7 +691,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="43">
+  <cellStyles count="45">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -697,11 +720,13 @@
     <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
     <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
     <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
     <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
     <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
     <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
     <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
     <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
@@ -1012,26 +1037,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AQ15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="8" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.83203125" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="38" width="11" style="1" bestFit="1" customWidth="1"/>
-    <col min="39" max="43" width="9" style="1" bestFit="1" customWidth="1"/>
-    <col min="44" max="16384" width="9.140625" style="1"/>
+    <col min="4" max="4" width="5.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="38" width="12.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="39" max="43" width="10.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="44" max="16384" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:43">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -1162,7 +1187,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:43">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -1295,7 +1320,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:43">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -1428,7 +1453,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:43">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -1561,7 +1586,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:43">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -1694,7 +1719,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:43">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -1827,7 +1852,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:43">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -1960,7 +1985,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:43">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -2093,7 +2118,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:43">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -2226,7 +2251,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:43">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -2359,7 +2384,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:43">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -2492,7 +2517,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:43">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -2625,7 +2650,7 @@
         <v>8.5000000000000006E-3</v>
       </c>
     </row>
-    <row r="13" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:43">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -2758,7 +2783,7 @@
         <v>9.7600000000000006E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:43">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -2891,7 +2916,7 @@
         <v>3.9199999999999999E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:43">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -3026,6 +3051,11 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>